<commit_message>
Updated data and removed max,min, avg tags
</commit_message>
<xml_diff>
--- a/src/assets/data/Data-ControlSystemv1.1.xlsx
+++ b/src/assets/data/Data-ControlSystemv1.1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Y1" sheetId="1" r:id="rId1"/>
@@ -2492,8 +2492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3394,7 +3394,7 @@
         <v>423</v>
       </c>
       <c r="C26">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D26">
         <v>82</v>
@@ -3426,7 +3426,7 @@
         <v>70</v>
       </c>
       <c r="C27">
-        <v>418</v>
+        <v>425</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3434,7 +3434,7 @@
         <v>71</v>
       </c>
       <c r="C28">
-        <v>415</v>
+        <v>423</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -3442,7 +3442,7 @@
         <v>72</v>
       </c>
       <c r="C29">
-        <v>410</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -3450,7 +3450,7 @@
         <v>73</v>
       </c>
       <c r="C30">
-        <v>405</v>
+        <v>425</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -3458,7 +3458,7 @@
         <v>74</v>
       </c>
       <c r="C31">
-        <v>401</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -4290,7 +4290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>